<commit_message>
second fase (wikipedia api and nlp topic models and cotizacion)
</commit_message>
<xml_diff>
--- a/Data/Conversation Chart Flow.xlsx
+++ b/Data/Conversation Chart Flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\ai_chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B6382F-FC4A-4F6D-B9E3-F3D39B8654E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49F4B21-9D7F-49EA-94F2-0E3B71ECB5A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C508BC11-13A6-481C-8C9D-92C2A7B204D8}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>Only Greeting</t>
   </si>
@@ -236,14 +236,6 @@
 OM: NA</t>
   </si>
   <si>
-    <t>Mensaje: Gracias por confiar en nosotros
-Migra a:
-Estado: 0
-Topic: NA
-Polarity: NA
-OM: NA</t>
-  </si>
-  <si>
     <t>Procesador de texto
 (Si recibe un mensaje con estado 1 y Topic = selcted topics (ST) )
 (anliza solo respuesta)</t>
@@ -369,6 +361,82 @@
     <t xml:space="preserve">Aca se debe procesar OM ya diferente por tema
 (por ahora mensaje de despedida)
 </t>
+  </si>
+  <si>
+    <t>No Topic</t>
+  </si>
+  <si>
+    <t>Catch Error</t>
+  </si>
+  <si>
+    <t>Mensaje:  Hmm.. Este tema es relativo a ACTUARIA? O es de otro tema?
+Migra a:
+Estado: 1
+Topic: NT
+Polarity: NA
+OM: __</t>
+  </si>
+  <si>
+    <t>Mensaje: Gracias por contactarnos, si desea deje su correo y/o numero de telefono y nos contactaremos con usted.
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
+  </si>
+  <si>
+    <t>Procesador de texto
+(Si recibe un mensaje con estado 1 y Topic = NT )
+(anliza solo respuesta)</t>
+  </si>
+  <si>
+    <t>ACTUARIA</t>
+  </si>
+  <si>
+    <t>Otro Tema</t>
+  </si>
+  <si>
+    <t>Pregunta: No entendi su respuesta, el tema es relativo a ACTUARIA o a otro tema?
+Migra a:
+Estado: 1
+Topic: maintain equal
+Polarity: maintain equal
+OM: maintain equal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mensaje: Lo que se de este tema es: Query Wikipedia
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA
+</t>
+  </si>
+  <si>
+    <t>Procesador de texto
+(Si recibe un mensaje con estado 1 y Queja)
+(anlizar solo respuesta)</t>
+  </si>
+  <si>
+    <t>Procesador de texto
+(Si recibe un mensaje con estado 4 y ST)
+(respuesta)</t>
+  </si>
+  <si>
+    <t>Mensaje: Muchas gracias, nos contactaremos con usted en la brevedad posible
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
+  </si>
+  <si>
+    <t>Mensaje: Gracias por confiar en nosotros!
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
   </si>
 </sst>
 </file>
@@ -2906,15 +2974,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:colOff>1057275</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2928,9 +2996,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1419860" y="7526020"/>
-          <a:ext cx="38100" cy="1165860"/>
+        <a:xfrm>
+          <a:off x="1454150" y="8661400"/>
+          <a:ext cx="3175" cy="587375"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2959,15 +3027,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:colOff>1076325</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:colOff>1079500</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2981,9 +3049,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4089400" y="7536180"/>
-          <a:ext cx="38100" cy="1181100"/>
+        <a:xfrm flipH="1">
+          <a:off x="4076700" y="8667750"/>
+          <a:ext cx="3175" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3688,10 +3756,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>1151467</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>8468</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3706,8 +3774,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4140200" y="3848100"/>
-          <a:ext cx="23439967" cy="8468"/>
+          <a:off x="4130675" y="3781425"/>
+          <a:ext cx="26044525" cy="9525"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4638,6 +4706,471 @@
         <a:xfrm>
           <a:off x="11933904" y="20746065"/>
           <a:ext cx="0" cy="248265"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1193800</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="49" name="Straight Arrow Connector 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C94EF9F3-2BAF-47B6-BF7B-12898E7A79F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="32775525" y="3781425"/>
+          <a:ext cx="12700" cy="1500717"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52404D31-52C6-4350-A3B4-8555AA3FEFA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11817350" y="8667750"/>
+          <a:ext cx="12700" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFAAE22-411A-4E0F-958A-7254A140A0EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14420850" y="8680450"/>
+          <a:ext cx="25400" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1137920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1163320</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>73660</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7442A743-F8A9-4777-B7F5-BF3655A7AC96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17130395" y="8658860"/>
+          <a:ext cx="25400" cy="596900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Straight Connector 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EF27284-DE4A-4235-A988-31C2C21663F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11817350" y="8661400"/>
+          <a:ext cx="5318125" cy="6350"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BB43FC6-6A67-402A-B556-D62491485430}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14433550" y="8350250"/>
+          <a:ext cx="0" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1155700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Arrow Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B85FD97-B5A0-4DE5-B622-4D1191C8122F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="27536775" y="7162800"/>
+          <a:ext cx="12700" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1081548</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>12290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1081548</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>24581</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Straight Connector 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB81F3B8-2F4D-4210-B9AC-10A3276CC13D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11901948" y="20724835"/>
+          <a:ext cx="0" cy="552619"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1106130</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>122904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1106130</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>27040</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Straight Connector 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90417C03-F66A-4182-8101-62ADD41CA716}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11926530" y="19588540"/>
+          <a:ext cx="0" cy="264355"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4962,7 +5495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C6BDDDA-C780-4646-B0AF-3939A885ED1A}">
   <dimension ref="B3:R38"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5165,10 +5698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDF1F2F-960D-43E5-8918-BCC079E49472}">
-  <dimension ref="B4:V63"/>
+  <dimension ref="B4:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="N19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5197,33 +5730,35 @@
     <col min="22" max="22" width="32.109375" style="2" customWidth="1"/>
     <col min="23" max="23" width="5.88671875" style="2" customWidth="1"/>
     <col min="24" max="24" width="32.109375" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="8.88671875" style="2"/>
+    <col min="25" max="25" width="5.77734375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="32.109375" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:22" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:24" ht="69" x14ac:dyDescent="0.3">
       <c r="P4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:24" x14ac:dyDescent="0.3">
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:24" x14ac:dyDescent="0.3">
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="4:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:22" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:24" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:24" x14ac:dyDescent="0.3">
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:24" x14ac:dyDescent="0.3">
       <c r="P10" s="4"/>
     </row>
-    <row r="12" spans="4:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -5235,7 +5770,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="16" spans="4:22" s="7" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:24" s="7" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="3" t="s">
         <v>28</v>
       </c>
@@ -5259,26 +5794,29 @@
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D18" s="6"/>
     </row>
-    <row r="20" spans="2:22" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:24" ht="124.2" x14ac:dyDescent="0.3">
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -5294,34 +5832,40 @@
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="L21" s="6"/>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="L22" s="6"/>
     </row>
-    <row r="23" spans="2:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:22" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:24" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D24" s="8" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="L24" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="V24" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -5334,8 +5878,17 @@
       <c r="N27" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="T27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>5</v>
       </c>
@@ -5349,10 +5902,12 @@
       </c>
       <c r="K28" s="5"/>
       <c r="M28" s="5"/>
-    </row>
-    <row r="31" spans="2:22" ht="165.6" x14ac:dyDescent="0.3">
+      <c r="U28" s="5"/>
+      <c r="W28" s="5"/>
+    </row>
+    <row r="31" spans="2:24" ht="165.6" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="1" t="s">
@@ -5360,32 +5915,43 @@
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K31" s="7"/>
       <c r="L31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M31" s="7"/>
       <c r="N31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U31" s="7"/>
+      <c r="V31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W31" s="7"/>
+      <c r="X31" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:18" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="2:18" ht="110.4" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L39" s="7" t="s">
         <v>32</v>
@@ -5422,10 +5988,10 @@
     </row>
     <row r="43" spans="2:18" ht="112.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L43" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O43" s="10"/>
       <c r="P43" s="6"/>
@@ -5455,10 +6021,10 @@
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.3">
       <c r="J47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N47" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="N47" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
@@ -5477,10 +6043,10 @@
     </row>
     <row r="51" spans="8:16" ht="96.6" x14ac:dyDescent="0.3">
       <c r="J51" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="8:16" x14ac:dyDescent="0.3">
@@ -5497,7 +6063,7 @@
     </row>
     <row r="55" spans="8:16" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J55" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N55" s="6"/>
     </row>
@@ -5520,15 +6086,37 @@
     </row>
     <row r="63" spans="8:16" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H63" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I63" s="7"/>
       <c r="J63" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K63" s="7"/>
       <c r="L63" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="8:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="8:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H67" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H68" s="6"/>
+    </row>
+    <row r="71" spans="8:8" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="H71" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integracion en el flow con AZURE
</commit_message>
<xml_diff>
--- a/Data/Conversation Chart Flow.xlsx
+++ b/Data/Conversation Chart Flow.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\ai_chatbot\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\chatbot\ai_chatbot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448B98F-4D7B-4A69-8716-2664EC3CB86E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C20F3-C00C-4548-8E8A-99B5A34C45ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C508BC11-13A6-481C-8C9D-92C2A7B204D8}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="81">
   <si>
     <t>Only Greeting</t>
   </si>
@@ -205,13 +205,6 @@
     <t>Hi Five</t>
   </si>
   <si>
-    <t>Jubilacion Patronal
-Renuncia/Despido/Desahucio
-IESS
-Otros servicios (Charlas/Capaci./Financiera)
-Consultoria</t>
-  </si>
-  <si>
     <t>Contacto</t>
   </si>
   <si>
@@ -315,42 +308,12 @@
 OM: maintain equal</t>
   </si>
   <si>
-    <t>Pregunta: Requiere el envio de una cotizacion?
-Migra a:
-Estado: 3
-Topic: maintain equal
-Polarity: maintain equal
-OM: maintain equal</t>
-  </si>
-  <si>
-    <t>Procesador de texto
-(Si recibe un mensaje con estado 3 y ST)
-(respuesta)</t>
-  </si>
-  <si>
     <t>Mensaje: Perfecto, nos puede dejar un nombre y un correo para contactarnos y enviar la propuesta de {Tema}?
 Migra a:
 Estado: 4
 Topic: maintain equal
 Polarity: maintain equal
 OM: maintain equal</t>
-  </si>
-  <si>
-    <t>Pregunta: No entendi su respuesta, requiere envio de una cotizacion?
-Migra a:
-Estado: 3
-Topic: maintain equal
-Polarity: maintain equal
-OM: maintain equal</t>
-  </si>
-  <si>
-    <t>Se debe unir con negativo cotizacion
-(por ahora mensaje de despedida)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aca se debe procesar OM ya diferente por tema
-(por ahora mensaje de despedida)
-</t>
   </si>
   <si>
     <t>No Topic</t>
@@ -439,17 +402,110 @@
     <t>Curr_Proc_Info</t>
   </si>
   <si>
-    <t>General_Info</t>
-  </si>
-  <si>
-    <t>Query a una base (kohinor)</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Jubilacion Patronal
+Renuncia/Despido/Desahucio
+IESS
+Consultoria</t>
+  </si>
+  <si>
+    <t>Otros servicios (Charlas/Capaci./Financiera)</t>
+  </si>
+  <si>
+    <t>Estado 0</t>
+  </si>
+  <si>
+    <t>Estado 1</t>
+  </si>
+  <si>
+    <t>Estado 2</t>
+  </si>
+  <si>
+    <t>Estado 3</t>
+  </si>
+  <si>
+    <t>Estado 4</t>
+  </si>
+  <si>
+    <t>Pregunta: Requiere el envio de una cotizacion?
+Migra a:
+Estado: 3
+Topic: maintain equal
+Polarity: maintain equal
+OM: maintain equal
+Intent: Cotizacion</t>
+  </si>
+  <si>
+    <t>Procesador de texto
+(Si recibe un mensaje con estado 3 y ST y Cotizacion)
+(respuesta)</t>
+  </si>
+  <si>
+    <t>Procesador de texto
+(Si recibe un mensaje con estado 3 y ST y Curr_Proc_Info)
+(respuesta)</t>
+  </si>
+  <si>
+    <t>Pregunta: Requiere informacion sobre un proceso que actualmente esta realizando con ACTUARIA?
+Migra a:
+Estado: 3
+Topic: maintain equal
+Polarity: maintain equal
+OM: maintain equal
+Intent: Curr_Proc_Info</t>
+  </si>
+  <si>
+    <t>No se encontro intent, Hasta aca nomas esta hecho
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
+  </si>
+  <si>
+    <t>Aqui se debe hacer una consulta al API de KOHINOR</t>
+  </si>
+  <si>
+    <t>Pregunta: No entendi su respuesta, requiere envio de una cotizacion?
+Migra a:
+Estado: 3
+Topic: maintain equal
+Polarity: maintain equal
+OM: maintain equal
+Intent: Cotizacion</t>
+  </si>
+  <si>
+    <t>Mensaje: Para charlas hay que desarrollar la info de horarios, hasta aca nomas esta hecho
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
+  </si>
+  <si>
+    <t>No se encontro intent, Hasta aca nomas esta hecho (se puede unir con estado anterior)
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA
+Intent: NA</t>
+  </si>
+  <si>
+    <t>No se encontro intent, Hasta aca nomas esta hecho (se puede unir con estado anterior)
+Migra a:
+Estado: 0
+Topic: NA
+Polarity: NA
+OM: NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +515,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -515,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -546,6 +617,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2407,13 +2485,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1049020</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
@@ -2460,13 +2538,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>787400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -2535,13 +2613,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -2587,13 +2665,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -2637,13 +2715,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>977900</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -2690,13 +2768,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>965200</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1003300</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -2743,13 +2821,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2796,13 +2874,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -2849,13 +2927,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>241300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1676400</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>787400</xdr:rowOff>
@@ -2930,13 +3008,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>495300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>514350</xdr:rowOff>
@@ -2982,13 +3060,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1057275</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
@@ -3035,13 +3113,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1076325</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1079500</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -3088,13 +3166,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1104900</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1130300</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -3141,13 +3219,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -3194,13 +3272,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -3247,13 +3325,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1137920</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1163320</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>73660</xdr:rowOff>
@@ -3300,13 +3378,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>1066800</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3350,13 +3428,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1066800</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
@@ -3400,13 +3478,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3450,13 +3528,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -3500,13 +3578,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -3553,13 +3631,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -3606,13 +3684,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1192161</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>159774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1229032</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>135193</xdr:rowOff>
@@ -3659,13 +3737,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>965200</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -3709,13 +3787,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1168400</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1168400</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -3759,16 +3837,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>1181100</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3782,9 +3860,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4130675" y="3781425"/>
-          <a:ext cx="26044525" cy="9525"/>
+        <a:xfrm flipV="1">
+          <a:off x="4178300" y="3962400"/>
+          <a:ext cx="36664900" cy="38100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3809,13 +3887,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1003300</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -3859,13 +3937,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3912,13 +3990,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1130300</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -3965,13 +4043,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1066800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1079500</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
@@ -4018,13 +4096,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1155291</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>1231900</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>12291</xdr:rowOff>
@@ -4068,13 +4146,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -4118,13 +4196,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1118419</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1155290</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>147483</xdr:rowOff>
@@ -4171,13 +4249,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1056967</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>73742</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>1069667</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>99142</xdr:rowOff>
@@ -4224,13 +4302,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1079500</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1117600</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -4277,13 +4355,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1104900</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1130300</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
@@ -4330,16 +4408,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1253613</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>12293</xdr:rowOff>
+      <xdr:rowOff>12295</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4354,8 +4432,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12054963" y="17049750"/>
-          <a:ext cx="15624687" cy="12293"/>
+          <a:off x="23542113" y="19069050"/>
+          <a:ext cx="15700887" cy="12295"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4380,13 +4458,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>958645</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>36871</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>958645</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>113071</xdr:rowOff>
@@ -4430,13 +4508,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1241322</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1241323</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>86032</xdr:rowOff>
@@ -4483,13 +4561,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1072025</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>21816</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>1084313</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>157009</xdr:rowOff>
@@ -4536,13 +4614,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1106129</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>12291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>1118419</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>24581</xdr:rowOff>
@@ -4586,13 +4664,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1106129</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>12291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1144229</xdr:colOff>
       <xdr:row>61</xdr:row>
       <xdr:rowOff>126591</xdr:rowOff>
@@ -4639,13 +4717,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1081548</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>12290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1081548</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>24581</xdr:rowOff>
@@ -4689,13 +4767,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1106130</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>122904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>1106130</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>27040</xdr:rowOff>
@@ -4739,13 +4817,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>1181100</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>1193800</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>110067</xdr:rowOff>
@@ -4792,13 +4870,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -4845,13 +4923,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1054100</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4898,13 +4976,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>1137920</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>1163320</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>73660</xdr:rowOff>
@@ -4951,13 +5029,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>1016000</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5001,13 +5079,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1041400</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -5051,13 +5129,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1155700</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>92075</xdr:rowOff>
@@ -5104,13 +5182,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1081548</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>12290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1081548</xdr:colOff>
       <xdr:row>70</xdr:row>
       <xdr:rowOff>24581</xdr:rowOff>
@@ -5154,13 +5232,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1106130</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>122904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>1106130</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>27040</xdr:rowOff>
@@ -5204,13 +5282,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1276350</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>1288638</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>135193</xdr:rowOff>
@@ -5237,6 +5315,368 @@
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>996950</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Straight Arrow Connector 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF149F93-E9DB-44D8-AC24-F7CA97E88454}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11836400" y="3765550"/>
+          <a:ext cx="12700" cy="1612900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1117600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Straight Arrow Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2029D72D-BC84-4FF1-8872-233C5B93407B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23368000" y="23869650"/>
+          <a:ext cx="38100" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1130300</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Straight Arrow Connector 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D6A9995-2097-4BF7-8F39-5540BDF2A951}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26003250" y="23895050"/>
+          <a:ext cx="25400" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1106129</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>12291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>1118419</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>24581</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Connector 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D590E24-ECBF-43B2-953C-51212AAA985F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20784779" y="23881941"/>
+          <a:ext cx="5231990" cy="12290"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1106129</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>12291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1144229</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>126591</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Straight Arrow Connector 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E33400DB-94C1-46F6-8BE7-0304DA1069EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20784779" y="23881941"/>
+          <a:ext cx="38100" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1081548</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>12290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1081548</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>24581</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Straight Connector 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81591DF5-F0F3-4D27-B322-E6369A8B2F18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23370048" y="23196140"/>
+          <a:ext cx="0" cy="698091"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1106130</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>122904</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1106130</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>27040</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Straight Connector 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C8F8C5D-C8A9-44F8-808C-58EDFD7AC911}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23394630" y="21916104"/>
+          <a:ext cx="0" cy="361336"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -5760,68 +6200,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDF1F2F-960D-43E5-8918-BCC079E49472}">
-  <dimension ref="B4:X71"/>
+  <dimension ref="A4:AM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="32.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="32.109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="32.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="5.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="32.109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.88671875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="32.109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="5.88671875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="32.109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="32.109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="5.88671875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="32.109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="5.77734375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="32.109375" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="14.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="32.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="32.109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="32.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="32.109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.88671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="32.109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.88671875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="32.109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="5.88671875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="32.109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="5.88671875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="32.109375" style="2" customWidth="1"/>
+    <col min="24" max="24" width="5.88671875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="32.109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="5.77734375" style="2" customWidth="1"/>
+    <col min="27" max="27" width="32.109375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="5.77734375" style="2" customWidth="1"/>
+    <col min="29" max="29" width="32.21875" style="2" customWidth="1"/>
+    <col min="30" max="30" width="5.77734375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="32.21875" style="2" customWidth="1"/>
+    <col min="32" max="32" width="5.77734375" style="2" customWidth="1"/>
+    <col min="33" max="33" width="32.21875" style="2" customWidth="1"/>
+    <col min="34" max="34" width="5.77734375" style="2" customWidth="1"/>
+    <col min="35" max="35" width="32.21875" style="2" customWidth="1"/>
+    <col min="36" max="36" width="5.77734375" style="2" customWidth="1"/>
+    <col min="37" max="37" width="32.21875" style="2" customWidth="1"/>
+    <col min="38" max="38" width="5.77734375" style="2" customWidth="1"/>
+    <col min="39" max="39" width="32.21875" style="2" customWidth="1"/>
+    <col min="40" max="40" width="5.77734375" style="2" customWidth="1"/>
+    <col min="41" max="41" width="32.21875" style="2" customWidth="1"/>
+    <col min="42" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:24" ht="69" x14ac:dyDescent="0.3">
-      <c r="P4" s="1" t="s">
-        <v>34</v>
+    <row r="4" spans="1:33" ht="69" x14ac:dyDescent="0.35">
+      <c r="Q4" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="P5" s="3"/>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="P6" s="3"/>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="4:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:24" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="P8" s="8" t="s">
+    <row r="7" spans="1:33" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:33" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="P9" s="4"/>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="P10" s="4"/>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="Q10" s="4"/>
     </row>
-    <row r="12" spans="4:24" x14ac:dyDescent="0.3">
-      <c r="D12" s="7"/>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -5831,360 +6288,441 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
     </row>
-    <row r="16" spans="4:24" s="7" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="3" t="s">
+    <row r="16" spans="1:33" s="7" customFormat="1" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="K16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="L16" s="3" t="s">
+      <c r="S16" s="2"/>
+      <c r="U16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W16" s="2"/>
+      <c r="Y16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N16" s="2"/>
-      <c r="P16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="7" t="s">
+      <c r="AC16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG16" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E18" s="6"/>
+    </row>
+    <row r="20" spans="1:33" ht="124.2" x14ac:dyDescent="0.35">
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="Y20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="U21" s="6"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="U22" s="6"/>
+    </row>
+    <row r="23" spans="1:33" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="1:33" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="U24" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE24" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG27" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="C28" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="T28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AF28" s="5"/>
+    </row>
+    <row r="31" spans="1:33" ht="165.6" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T31" s="7"/>
+      <c r="U31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V31" s="7"/>
+      <c r="W31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="1:39" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="U35" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" ht="110.4" x14ac:dyDescent="0.35">
+      <c r="C39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U39" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="T16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="X16" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="9"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="9"/>
     </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D17" s="6"/>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="10"/>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D18" s="6"/>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="W41" s="10"/>
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
     </row>
-    <row r="20" spans="2:24" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="D20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="1" t="s">
+    <row r="42" spans="1:39" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="W42" s="10"/>
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+    </row>
+    <row r="43" spans="1:39" ht="112.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="W43" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="P20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U20" s="7"/>
-      <c r="V20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="X43" s="10"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="10"/>
     </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L21" s="6"/>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="W44" s="10"/>
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="10"/>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="L22" s="6"/>
+    <row r="45" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="W45" s="10"/>
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="10"/>
     </row>
-    <row r="23" spans="2:24" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:24" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="8" t="s">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="W46" s="10"/>
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="10"/>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="S47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="W47" s="5"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="L24" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="V24" s="8" t="s">
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="10"/>
+      <c r="AE47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI47" s="10"/>
+      <c r="AJ47" s="10"/>
+      <c r="AK47" s="11"/>
+      <c r="AL47" s="10"/>
+      <c r="AM47" s="10"/>
+    </row>
+    <row r="48" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="X48" s="10"/>
+      <c r="Y48" s="10"/>
+      <c r="Z48" s="10"/>
+      <c r="AA48" s="10"/>
+      <c r="AI48" s="10"/>
+      <c r="AJ48" s="10"/>
+      <c r="AK48" s="10"/>
+      <c r="AL48" s="10"/>
+      <c r="AM48" s="10"/>
+    </row>
+    <row r="49" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="AI49" s="10"/>
+      <c r="AJ49" s="10"/>
+      <c r="AK49" s="10"/>
+      <c r="AL49" s="10"/>
+      <c r="AM49" s="10"/>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="X50" s="10"/>
+      <c r="Y50" s="10"/>
+      <c r="AI50" s="10"/>
+      <c r="AJ50" s="10"/>
+      <c r="AK50" s="10"/>
+      <c r="AL50" s="10"/>
+      <c r="AM50" s="10"/>
+    </row>
+    <row r="51" spans="1:39" ht="124.2" x14ac:dyDescent="0.35">
+      <c r="S51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AI51" s="10"/>
+      <c r="AJ51" s="10"/>
+      <c r="AK51" s="6"/>
+      <c r="AL51" s="10"/>
+      <c r="AM51" s="10"/>
+    </row>
+    <row r="52" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="S52" s="6"/>
+      <c r="Y52" s="6"/>
+      <c r="AI52" s="10"/>
+      <c r="AJ52" s="10"/>
+      <c r="AK52" s="10"/>
+      <c r="AL52" s="10"/>
+      <c r="AM52" s="10"/>
+    </row>
+    <row r="53" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="S53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="AI53" s="10"/>
+      <c r="AJ53" s="10"/>
+      <c r="AK53" s="10"/>
+      <c r="AL53" s="10"/>
+      <c r="AM53" s="10"/>
+    </row>
+    <row r="54" spans="1:39" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S54" s="6"/>
+      <c r="Y54" s="6"/>
+    </row>
+    <row r="55" spans="1:39" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="S55" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y55" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="S56" s="6"/>
+      <c r="Y56" s="6"/>
+    </row>
+    <row r="60" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="Q60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W60" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="X60" s="7"/>
+      <c r="Y60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z60" s="7"/>
+      <c r="AA60" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:39" ht="124.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R63" s="7"/>
+      <c r="S63" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T63" s="7"/>
+      <c r="U63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="W63" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="X63" s="7"/>
+      <c r="Y63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z63" s="7"/>
+      <c r="AA63" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="Q64" s="6"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q65" s="6"/>
+    </row>
+    <row r="66" spans="1:17" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q66" s="6"/>
+    </row>
+    <row r="67" spans="1:17" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q67" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D25" s="3"/>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q68" s="6"/>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="T27" s="7" t="s">
+    <row r="71" spans="1:17" ht="110.4" x14ac:dyDescent="0.35">
+      <c r="Q71" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="V27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="X27" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="W28" s="5"/>
-    </row>
-    <row r="31" spans="2:24" ht="165.6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K31" s="7"/>
-      <c r="L31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M31" s="7"/>
-      <c r="N31" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U31" s="7"/>
-      <c r="V31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W31" s="7"/>
-      <c r="X31" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="2:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="2:22" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="2:22" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L39" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="O39" s="10"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="10"/>
-      <c r="R39" s="9"/>
-    </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-    </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="N41" s="10"/>
-      <c r="O41" s="10"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="10"/>
-      <c r="R41" s="10"/>
-    </row>
-    <row r="42" spans="2:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-    </row>
-    <row r="43" spans="2:22" ht="112.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L43" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="O43" s="10"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-    </row>
-    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="N44" s="10"/>
-      <c r="O44" s="10"/>
-      <c r="P44" s="10"/>
-      <c r="Q44" s="10"/>
-      <c r="R44" s="10"/>
-    </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="N45" s="10"/>
-      <c r="O45" s="10"/>
-      <c r="P45" s="10"/>
-      <c r="Q45" s="10"/>
-      <c r="R45" s="10"/>
-    </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="N46" s="10"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-    </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="J47" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="N47" s="5"/>
-      <c r="O47" s="10"/>
-      <c r="P47" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q47" s="10"/>
-      <c r="R47" s="10"/>
-      <c r="V47" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="O48" s="10"/>
-      <c r="P48" s="10"/>
-      <c r="Q48" s="10"/>
-      <c r="R48" s="10"/>
-    </row>
-    <row r="50" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="O50" s="10"/>
-      <c r="P50" s="10"/>
-    </row>
-    <row r="51" spans="8:22" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="J51" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="V51" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="J52" s="6"/>
-      <c r="N52" s="6"/>
-    </row>
-    <row r="53" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="J53" s="6"/>
-      <c r="N53" s="6"/>
-    </row>
-    <row r="54" spans="8:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J54" s="6"/>
-      <c r="N54" s="6"/>
-    </row>
-    <row r="55" spans="8:22" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J55" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N55" s="6"/>
-    </row>
-    <row r="56" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="J56" s="6"/>
-      <c r="N56" s="6"/>
-    </row>
-    <row r="60" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="H60" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="8:22" ht="124.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H63" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I63" s="7"/>
-      <c r="J63" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="K63" s="7"/>
-      <c r="L63" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="8:22" x14ac:dyDescent="0.3">
-      <c r="H64" s="6"/>
-    </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H65" s="6"/>
-    </row>
-    <row r="66" spans="8:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H66" s="6"/>
-    </row>
-    <row r="67" spans="8:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H67" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H68" s="6"/>
-    </row>
-    <row r="71" spans="8:8" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="H71" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>